<commit_message>
update to KiCad8, DNP 32KHz crystal, update BOM
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeSupra BOM.xlsx
+++ b/Manufacturing Files/bitaxeSupra BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitaxe/bitaxe-401/Manufacturing Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC24B48F-08D9-C244-8214-3C3CCF2C3EB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6555D4-7A4E-5644-83F4-B953E9C0BCC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="27880" windowHeight="23940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="27880" windowHeight="23940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="173">
   <si>
     <t>Qty</t>
   </si>
@@ -89,18 +89,6 @@
     <t>865080345012</t>
   </si>
   <si>
-    <t>C30, C31</t>
-  </si>
-  <si>
-    <t>6.8pF</t>
-  </si>
-  <si>
-    <t>399-C0402C689C5GAC7867CT-ND</t>
-  </si>
-  <si>
-    <t>C0402C689C5GAC7867</t>
-  </si>
-  <si>
     <t>C34, C36, C37</t>
   </si>
   <si>
@@ -552,18 +540,6 @@
   </si>
   <si>
     <t>ESP32-S3-WROOM-1-N16R8</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>32.768kHz</t>
-  </si>
-  <si>
-    <t>728-1074-1-ND</t>
-  </si>
-  <si>
-    <t>SC32S-7PF20PPM</t>
   </si>
 </sst>
 </file>
@@ -954,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1057,7 +1033,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -1074,19 +1050,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1094,10 +1070,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
       </c>
       <c r="D8" t="s">
         <v>31</v>
@@ -1142,7 +1118,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
@@ -1159,7 +1135,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>45</v>
@@ -1182,13 +1158,13 @@
         <v>49</v>
       </c>
       <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
         <v>50</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>51</v>
-      </c>
-      <c r="E13" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1196,10 +1172,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
         <v>53</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
       </c>
       <c r="D14" t="s">
         <v>54</v>
@@ -1222,7 +1198,7 @@
         <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1230,16 +1206,16 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
         <v>60</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>61</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>62</v>
-      </c>
-      <c r="E16" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1267,13 +1243,13 @@
         <v>67</v>
       </c>
       <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
         <v>68</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>69</v>
-      </c>
-      <c r="E18" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1281,10 +1257,10 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
         <v>71</v>
-      </c>
-      <c r="C19" t="s">
-        <v>64</v>
       </c>
       <c r="D19" t="s">
         <v>72</v>
@@ -1295,7 +1271,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
         <v>74</v>
@@ -1307,29 +1283,29 @@
         <v>76</v>
       </c>
       <c r="E20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
         <v>78</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>79</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>80</v>
-      </c>
-      <c r="E21" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
         <v>81</v>
@@ -1346,7 +1322,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
         <v>85</v>
@@ -1363,7 +1339,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
         <v>89</v>
@@ -1380,7 +1356,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
         <v>93</v>
@@ -1428,6 +1404,9 @@
       <c r="E27" t="s">
         <v>104</v>
       </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -1445,9 +1424,6 @@
       <c r="E28" t="s">
         <v>108</v>
       </c>
-      <c r="F28" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -1525,13 +1501,13 @@
         <v>125</v>
       </c>
       <c r="C33" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="D33" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="E33" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1539,21 +1515,21 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" t="s">
+        <v>128</v>
+      </c>
+      <c r="E34" t="s">
         <v>129</v>
-      </c>
-      <c r="C34" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" t="s">
-        <v>107</v>
-      </c>
-      <c r="E34" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
         <v>130</v>
@@ -1570,7 +1546,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B36" t="s">
         <v>134</v>
@@ -1599,7 +1575,7 @@
         <v>140</v>
       </c>
       <c r="E37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1607,16 +1583,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>141</v>
+      </c>
+      <c r="C38" t="s">
         <v>142</v>
-      </c>
-      <c r="C38" t="s">
-        <v>143</v>
-      </c>
-      <c r="D38" t="s">
-        <v>144</v>
-      </c>
-      <c r="E38" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1624,9 +1594,15 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" t="s">
+        <v>144</v>
+      </c>
+      <c r="D39" t="s">
         <v>145</v>
       </c>
-      <c r="C39" t="s">
+      <c r="E39" t="s">
         <v>146</v>
       </c>
     </row>
@@ -1712,7 +1688,7 @@
         <v>165</v>
       </c>
       <c r="E44" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1720,16 +1696,16 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
+        <v>166</v>
+      </c>
+      <c r="C45" t="s">
         <v>167</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>168</v>
       </c>
-      <c r="D45" t="s">
-        <v>169</v>
-      </c>
       <c r="E45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1737,50 +1713,16 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" t="s">
         <v>170</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>171</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>172</v>
-      </c>
-      <c r="E46" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>173</v>
-      </c>
-      <c r="C47" t="s">
-        <v>174</v>
-      </c>
-      <c r="D47" t="s">
-        <v>175</v>
-      </c>
-      <c r="E47" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s">
-        <v>177</v>
-      </c>
-      <c r="C48" t="s">
-        <v>178</v>
-      </c>
-      <c r="D48" t="s">
-        <v>179</v>
-      </c>
-      <c r="E48" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1790,10 +1732,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1859,7 +1801,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -1870,13 +1812,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1884,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>31</v>
@@ -1914,7 +1856,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
@@ -1925,7 +1867,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>45</v>
@@ -1942,7 +1884,7 @@
         <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1950,7 +1892,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
         <v>54</v>
@@ -1972,10 +1914,10 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1997,7 +1939,7 @@
         <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2005,7 +1947,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
         <v>72</v>
@@ -2013,7 +1955,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
         <v>74</v>
@@ -2024,18 +1966,18 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
         <v>81</v>
@@ -2046,7 +1988,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
         <v>85</v>
@@ -2057,7 +1999,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
         <v>89</v>
@@ -2068,7 +2010,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
         <v>93</v>
@@ -2093,10 +2035,10 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2151,7 +2093,7 @@
         <v>125</v>
       </c>
       <c r="C32" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2159,15 +2101,15 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
         <v>130</v>
@@ -2178,7 +2120,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35" t="s">
         <v>134</v>
@@ -2203,10 +2145,10 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C37" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2269,10 +2211,10 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2280,32 +2222,10 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C44" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s">
-        <v>173</v>
-      </c>
-      <c r="C45" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="B46" t="s">
-        <v>177</v>
-      </c>
-      <c r="C46" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated BOM with R18 DNP
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeSupra BOM.xlsx
+++ b/Manufacturing Files/bitaxeSupra BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitaxe/bitaxe-401/Manufacturing Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Bitcoin/bitaxe/bitaxe-401/Manufacturing Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6555D4-7A4E-5644-83F4-B953E9C0BCC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0A86A1-90E9-9D49-88E4-27D7255E707F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="27880" windowHeight="23940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="27880" windowHeight="23940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="173">
   <si>
     <t>Qty</t>
   </si>
@@ -932,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1493,7 +1493,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1526,8 +1526,11 @@
       <c r="E34" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1544,7 +1547,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1561,7 +1564,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1578,7 +1581,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1589,7 +1592,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -1606,7 +1609,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -1623,7 +1626,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -1640,7 +1643,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -1657,7 +1660,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
@@ -1674,7 +1677,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
@@ -1691,7 +1694,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1</v>
       </c>
@@ -1708,7 +1711,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
@@ -1732,10 +1735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2098,24 +2101,24 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C33" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C34" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2123,10 +2126,10 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C35" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2134,10 +2137,10 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C36" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2145,10 +2148,10 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C37" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2156,10 +2159,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C38" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2167,10 +2170,10 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C39" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2178,10 +2181,10 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C40" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2189,10 +2192,10 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2200,10 +2203,10 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C42" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2211,20 +2214,9 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C43" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s">
-        <v>169</v>
-      </c>
-      <c r="C44" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>